<commit_message>
v1.2 verify that the previous comments modified
close publish audio wireframe review and verify the updates
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_PUBLISHAUDIO_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_PUBLISHAUDIO_REVIEWS.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Ahmed Abuzaid</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>28/4/2025</t>
   </si>
   <si>
@@ -125,12 +122,18 @@
   </si>
   <si>
     <t>edit the owner status of the sheet</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t>verify that the previous comments modified</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -695,7 +698,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -706,7 +709,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -754,10 +757,10 @@
     </row>
     <row r="2" spans="1:9" ht="75">
       <c r="A2" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>14</v>
@@ -766,27 +769,27 @@
         <v>13</v>
       </c>
       <c r="E2" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="22" t="s">
-        <v>23</v>
-      </c>
       <c r="G2" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="60">
       <c r="A3" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>14</v>
@@ -795,27 +798,27 @@
         <v>13</v>
       </c>
       <c r="E3" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="23" t="s">
-        <v>19</v>
-      </c>
       <c r="G3" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="90">
       <c r="A4" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>14</v>
@@ -824,27 +827,27 @@
         <v>13</v>
       </c>
       <c r="E4" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>27</v>
-      </c>
       <c r="G4" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" s="16" t="s">
         <v>31</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60">
       <c r="A5" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>14</v>
@@ -853,19 +856,19 @@
         <v>13</v>
       </c>
       <c r="E5" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="18" t="s">
+      <c r="I5" s="19" t="s">
         <v>31</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -964,7 +967,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -997,7 +1000,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="9">
         <v>45775</v>
@@ -1005,23 +1008,31 @@
     </row>
     <row r="3" spans="1:4" ht="18.75">
       <c r="A3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="D3" s="9">
         <v>45776</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
+    <row r="4" spans="1:4" ht="37.5">
+      <c r="A4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="9">
+        <v>45776</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>